<commit_message>
Power connector change + more comm ports
</commit_message>
<xml_diff>
--- a/Dragonflyte/Boards/Dragonflyte/Project Outputs for Dragonflyte/BOM/Dragonflyte.xlsx
+++ b/Dragonflyte/Boards/Dragonflyte/Project Outputs for Dragonflyte/BOM/Dragonflyte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="324">
   <si>
     <t>Designator</t>
   </si>
@@ -90,7 +90,7 @@
     <t>Bottom, Top</t>
   </si>
   <si>
-    <t>C5, C19, C68, C78, C83, C99, C100, C101, C102, C103, C104, C105, C107, C108, C110, C112, C113, C114, C117, C120, C121, C122, C123, C124, C125, C129, C132, C135, C139, C140, C141, C142, C143, C146, C149, C151, C152</t>
+    <t>C5, C19, C68, C78, C83, C99, C100, C101, C102, C103, C104, C105, C107, C108, C110, C112, C113, C114, C117, C120, C121, C122, C123, C124, C125, C129, C132, C135, C139, C140, C141, C142, C143, C146, C149, C151, C152, C158, C159, C160</t>
   </si>
   <si>
     <t>GRM155R70J104KA01D</t>
@@ -189,7 +189,7 @@
     <t>2.2uF 6.3V 20% 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>C81, C82, C88, C91, C92, C93, C94, C95, C96, C97, C98</t>
+    <t>C81, C82, C88, C91, C92, C93, C94, C95, C96, C97, C98, C162</t>
   </si>
   <si>
     <t>GRM155R70J105KA12D</t>
@@ -321,13 +321,16 @@
     <t>JP3</t>
   </si>
   <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>51296-3494</t>
-  </si>
-  <si>
-    <t>FFC-FPC-0.5</t>
+    <t>Hirose</t>
+  </si>
+  <si>
+    <t>BM28B0.6-40DS/2-0.35V(53)</t>
+  </si>
+  <si>
+    <t>BM28-0.35</t>
+  </si>
+  <si>
+    <t>Board to Board &amp; Mezzanine Connectors 40P Receptacle Straight SMT</t>
   </si>
   <si>
     <t>L1</t>
@@ -597,6 +600,15 @@
     <t>150R 0.063W 1% 0402 (1005 Metric)</t>
   </si>
   <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>RK73H1ETTP1200F</t>
+  </si>
+  <si>
+    <t>120R 0.063W 1% 0402 (1005 Metric)</t>
+  </si>
+  <si>
     <t>SW1, SW2</t>
   </si>
   <si>
@@ -889,6 +901,39 @@
   </si>
   <si>
     <t>TPS62097 2-A High Efficiency Step-Down Converter with iDCS Control, Forced PWM Mode and Selective Switching Frequency</t>
+  </si>
+  <si>
+    <t>U24</t>
+  </si>
+  <si>
+    <t>TCAN332DCNR</t>
+  </si>
+  <si>
+    <t>SOT-23-8</t>
+  </si>
+  <si>
+    <t>CAN Interface IC 3.3-V CAN Transceivers with CAN FD (Flexible Data Rate) 8-SOT-23 -40 to 125</t>
+  </si>
+  <si>
+    <t>U25</t>
+  </si>
+  <si>
+    <t>ADS112C04IRTET</t>
+  </si>
+  <si>
+    <t>IC ADC 16BIT I2C 1KSPS 16WQFN</t>
+  </si>
+  <si>
+    <t>U26</t>
+  </si>
+  <si>
+    <t>PCA9685BS,118</t>
+  </si>
+  <si>
+    <t>QFN-28</t>
+  </si>
+  <si>
+    <t>IC LED DRVR LIN DIM 25MA 28HVQFN</t>
   </si>
   <si>
     <t>Y1, Y3</t>
@@ -1295,7 +1340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1419,7 +1464,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -1679,7 +1724,7 @@
         <v>56</v>
       </c>
       <c r="B15" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
@@ -2029,7 +2074,7 @@
         <v>102</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>12</v>
@@ -2040,7 +2085,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -2049,13 +2094,13 @@
         <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>12</v>
@@ -2066,7 +2111,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B30" s="3">
         <v>4</v>
@@ -2075,13 +2120,13 @@
         <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>12</v>
@@ -2092,7 +2137,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B31" s="3">
         <v>2</v>
@@ -2101,13 +2146,13 @@
         <v>18</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>12</v>
@@ -2118,7 +2163,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
@@ -2127,13 +2172,13 @@
         <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>12</v>
@@ -2144,7 +2189,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
@@ -2153,13 +2198,13 @@
         <v>18</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>12</v>
@@ -2170,22 +2215,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>12</v>
@@ -2196,22 +2241,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>12</v>
@@ -2222,22 +2267,22 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>12</v>
@@ -2248,22 +2293,22 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B37" s="3">
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>12</v>
@@ -2274,22 +2319,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B38" s="3">
         <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>12</v>
@@ -2300,22 +2345,22 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B39" s="3">
         <v>8</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>12</v>
@@ -2326,22 +2371,22 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>12</v>
@@ -2352,22 +2397,22 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>12</v>
@@ -2378,22 +2423,22 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B42" s="3">
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>12</v>
@@ -2404,22 +2449,22 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B43" s="3">
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>12</v>
@@ -2430,22 +2475,22 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>12</v>
@@ -2456,22 +2501,22 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B45" s="3">
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>12</v>
@@ -2482,22 +2527,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>12</v>
@@ -2508,22 +2553,22 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>12</v>
@@ -2534,22 +2579,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B48" s="3">
         <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>12</v>
@@ -2560,22 +2605,22 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>12</v>
@@ -2586,22 +2631,22 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B50" s="3">
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>12</v>
@@ -2612,22 +2657,22 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>12</v>
@@ -2638,22 +2683,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>12</v>
@@ -2664,22 +2709,22 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>12</v>
@@ -2690,22 +2735,22 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>12</v>
@@ -2716,22 +2761,22 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>12</v>
@@ -2742,74 +2787,74 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B56" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="G56" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F57" s="2" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B58" s="3">
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>203</v>
+        <v>106</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>204</v>
+        <v>11</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>12</v>
@@ -2820,54 +2865,54 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B59" s="3">
-        <v>2</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="G59" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B60" s="3">
+        <v>2</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B60" s="3">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F60" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G60" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2887,59 +2932,59 @@
         <v>217</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>218</v>
+        <v>11</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B62" s="3">
-        <v>1</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>220</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B63" s="3">
         <v>1</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>224</v>
       </c>
       <c r="E63" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>12</v>
@@ -2956,13 +3001,13 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>11</v>
@@ -2971,27 +3016,27 @@
         <v>12</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B65" s="3">
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>232</v>
+        <v>11</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>12</v>
@@ -3008,16 +3053,16 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>12</v>
@@ -3028,22 +3073,22 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B67" s="3">
-        <v>1</v>
-      </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>12</v>
@@ -3054,22 +3099,22 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B68" s="3">
-        <v>1</v>
-      </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>12</v>
@@ -3080,13 +3125,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B69" s="3">
-        <v>1</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>249</v>
@@ -3101,7 +3146,7 @@
         <v>12</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3112,42 +3157,42 @@
         <v>1</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="G70" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B71" s="3">
-        <v>1</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="F71" s="2" t="s">
-        <v>11</v>
+        <v>260</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>12</v>
@@ -3158,65 +3203,65 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B72" s="3">
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>264</v>
+        <v>11</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B73" s="3">
-        <v>2</v>
-      </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="G73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B74" s="3">
+        <v>2</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B74" s="3">
-        <v>1</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>271</v>
@@ -3231,7 +3276,7 @@
         <v>12</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,7 +3287,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>275</v>
@@ -3268,16 +3313,16 @@
         <v>1</v>
       </c>
       <c r="C76" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>12</v>
@@ -3288,13 +3333,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B77" s="3">
-        <v>1</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>284</v>
@@ -3303,7 +3348,7 @@
         <v>285</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>11</v>
+        <v>286</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>12</v>
@@ -3314,28 +3359,28 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B78" s="3">
         <v>1</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>289</v>
+        <v>11</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3343,25 +3388,25 @@
         <v>290</v>
       </c>
       <c r="B79" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G79" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3372,16 +3417,16 @@
         <v>1</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="F80" s="2" t="s">
-        <v>11</v>
+        <v>297</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>12</v>
@@ -3392,54 +3437,54 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B81" s="3">
         <v>1</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>298</v>
+        <v>215</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>299</v>
       </c>
       <c r="E81" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="G81" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B82" s="3">
-        <v>1</v>
-      </c>
-      <c r="C82" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G82" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,7 +3492,7 @@
         <v>305</v>
       </c>
       <c r="B83" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>306</v>
@@ -3456,15 +3501,119 @@
         <v>307</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="F83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G83" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H83" s="2" t="s">
+      <c r="F84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B86" s="3">
+        <v>1</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>